<commit_message>
Securing (working) interim version
</commit_message>
<xml_diff>
--- a/Data/MeteoData/StationsData/sample_forecast_nowcast_8124.xlsx
+++ b/Data/MeteoData/StationsData/sample_forecast_nowcast_8124.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\LEG_analysis\Data\MeteoData\StationsData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F5246D1C-B2E7-430F-8251-A938C9D1F55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0282C369-B76C-4DAC-9AF7-B7A8AC94ECFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{C519F2D7-B74E-434C-8D02-3466116E1863}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{C519F2D7-B74E-434C-8D02-3466116E1863}"/>
   </bookViews>
   <sheets>
     <sheet name="sample_7day_forecast" sheetId="2" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="561">
   <si>
     <t>ForecastPeriod</t>
   </si>
@@ -1715,6 +1715,27 @@
   </si>
   <si>
     <t>NowcastPeriod { Time = 11/27/2025 5:15:00 AM, TemperatureC = 0.4, PrecipitationMm = 0, WindSpeedKmh = 3.8, WindGustsKmh = 6.8, SolarRadiationWm2 = 0, LocalTime = 11/27/2025 6:15:00 AM }</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>fit</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Filter</t>
   </si>
 </sst>
 </file>
@@ -1730,15 +1751,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1746,14 +1773,142 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1794,6 +1949,1621 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>value</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$12:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$Q$12:$Q$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FA3C-4FA6-9802-089ED1B5B7C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$12:$P$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$R$12:$R$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="52"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>179</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>197.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>215</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>232.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>246</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>257.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>272.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>276</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>277.5</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>275</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>272.5</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>265</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>255</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>187.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>165</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>142.5</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FA3C-4FA6-9802-089ED1B5B7C8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2027971936"/>
+        <c:axId val="87939551"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2027971936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="87939551"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="87939551"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2027971936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33DCBFF6-B025-DED8-E19F-F3D5BC8792E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2199,7 +3969,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01117122-E57D-4924-9BF0-323B8B11FEBD}">
   <dimension ref="A1:O169"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="F1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -10175,7 +11945,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85F52A60-9284-492B-994C-7021588A551F}">
   <dimension ref="A1:I361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -20669,13 +22441,2833 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2342C4DA-CFEA-4236-8A74-0524FEA4FF02}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C1" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="D1" s="11">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7">
+        <v>6</v>
+      </c>
+      <c r="J1" s="7">
+        <v>7</v>
+      </c>
+      <c r="K1" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D2" s="12">
+        <v>0</v>
+      </c>
+      <c r="E2" s="9">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9">
+        <v>15</v>
+      </c>
+      <c r="G2" s="9">
+        <v>25</v>
+      </c>
+      <c r="H2" s="9">
+        <v>25</v>
+      </c>
+      <c r="I2" s="9">
+        <v>15</v>
+      </c>
+      <c r="J2" s="9">
+        <v>10</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="9">
+        <v>5</v>
+      </c>
+      <c r="F3" s="9">
+        <v>15</v>
+      </c>
+      <c r="G3" s="9">
+        <v>30</v>
+      </c>
+      <c r="H3" s="9">
+        <v>30</v>
+      </c>
+      <c r="I3" s="9">
+        <v>15</v>
+      </c>
+      <c r="J3" s="9">
+        <v>5</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D4" s="12">
+        <v>2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>2</v>
+      </c>
+      <c r="F4" s="9">
+        <v>8</v>
+      </c>
+      <c r="G4" s="9">
+        <v>40</v>
+      </c>
+      <c r="H4" s="9">
+        <v>40</v>
+      </c>
+      <c r="I4" s="9">
+        <v>8</v>
+      </c>
+      <c r="J4" s="9">
+        <v>2</v>
+      </c>
+      <c r="K4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D5" s="13">
+        <v>3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3">
+        <v>43</v>
+      </c>
+      <c r="H5" s="3">
+        <v>43</v>
+      </c>
+      <c r="I5" s="3">
+        <v>6</v>
+      </c>
+      <c r="J5" s="3">
+        <v>1</v>
+      </c>
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="D7" s="6" t="s">
+        <v>557</v>
+      </c>
+      <c r="E7" s="7">
+        <v>-3</v>
+      </c>
+      <c r="F7" s="7">
+        <v>-2</v>
+      </c>
+      <c r="G7" s="7">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <v>2</v>
+      </c>
+      <c r="K7" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>560</v>
+      </c>
+      <c r="B8" s="14">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E8" s="3">
+        <f>VLOOKUP($B$8,$D$2:$K$5,E$1)</f>
+        <v>10</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" ref="F8:K8" si="0">VLOOKUP($B$8,$D$2:$K$5,F$1)</f>
+        <v>15</v>
+      </c>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="H8" s="3">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="J8" s="3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f>SUM(E8:K8)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="P11" t="s">
+        <v>554</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>555</v>
+      </c>
+      <c r="R11" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f>A12</f>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f t="shared" ref="P12:P14" si="1">B12</f>
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ref="Q12:Q14" si="2">C12</f>
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ref="R12:R14" si="3">M12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <f>A12</f>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <f>A12</f>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <f>A12</f>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f>VLOOKUP($B15+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <f>VLOOKUP($B15+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f>VLOOKUP($B15+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f>VLOOKUP($B15+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f>VLOOKUP($B15+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f>VLOOKUP($B15+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <f>VLOOKUP($B15+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <f>SUM(E15:K15)/M$8</f>
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <f>B15</f>
+        <v>4</v>
+      </c>
+      <c r="Q15">
+        <f>C15</f>
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <f>M15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <f>A16</f>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f>VLOOKUP($B16+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f>VLOOKUP($B16+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f>VLOOKUP($B16+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f>VLOOKUP($B16+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f>VLOOKUP($B16+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f>VLOOKUP($B16+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f>VLOOKUP($B16+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <f>SUM(E16:K16)/M$8</f>
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <f t="shared" ref="P16:P60" si="4">B16</f>
+        <v>5</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" ref="Q16:Q60" si="5">C16</f>
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <f t="shared" ref="R16:R60" si="6">M16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <f>A16</f>
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f>VLOOKUP($B17+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <f>VLOOKUP($B17+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <f>VLOOKUP($B17+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f>VLOOKUP($B17+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f>VLOOKUP($B17+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f>VLOOKUP($B17+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <f>VLOOKUP($B17+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <f>SUM(E17:K17)/M$8</f>
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <f>A16</f>
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f>VLOOKUP($B18+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <f>VLOOKUP($B18+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f>VLOOKUP($B18+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f>VLOOKUP($B18+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f>VLOOKUP($B18+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f>VLOOKUP($B18+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>400</v>
+      </c>
+      <c r="K18">
+        <f>VLOOKUP($B18+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f>SUM(E18:K18)/M$8</f>
+        <v>4</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <f>A16</f>
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <f>VLOOKUP($B19+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <f>VLOOKUP($B19+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <f>VLOOKUP($B19+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <f>VLOOKUP($B19+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <f>VLOOKUP($B19+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>600</v>
+      </c>
+      <c r="J19">
+        <f>VLOOKUP($B19+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>400</v>
+      </c>
+      <c r="K19">
+        <f>VLOOKUP($B19+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <f>SUM(E19:K19)/M$8</f>
+        <v>10</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>40</v>
+      </c>
+      <c r="B20">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <f>A20</f>
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <f>VLOOKUP($B20+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <f>VLOOKUP($B20+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f>VLOOKUP($B20+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <f>VLOOKUP($B20+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>1000</v>
+      </c>
+      <c r="I20">
+        <f>VLOOKUP($B20+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>600</v>
+      </c>
+      <c r="J20">
+        <f>VLOOKUP($B20+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>400</v>
+      </c>
+      <c r="K20">
+        <f>VLOOKUP($B20+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <f>SUM(E20:K20)/M$8</f>
+        <v>20</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21">
+        <f>A20</f>
+        <v>40</v>
+      </c>
+      <c r="E21">
+        <f>VLOOKUP($B21+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <f>VLOOKUP($B21+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>VLOOKUP($B21+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>1000</v>
+      </c>
+      <c r="H21">
+        <f>VLOOKUP($B21+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>1000</v>
+      </c>
+      <c r="I21">
+        <f>VLOOKUP($B21+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>600</v>
+      </c>
+      <c r="J21">
+        <f>VLOOKUP($B21+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>400</v>
+      </c>
+      <c r="K21">
+        <f>VLOOKUP($B21+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f>SUM(E21:K21)/M$8</f>
+        <v>30</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="R21">
+        <f t="shared" si="6"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>11</v>
+      </c>
+      <c r="C22">
+        <f>A20</f>
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <f>VLOOKUP($B22+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <f>VLOOKUP($B22+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>600</v>
+      </c>
+      <c r="G22">
+        <f>VLOOKUP($B22+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>1000</v>
+      </c>
+      <c r="H22">
+        <f>VLOOKUP($B22+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>1000</v>
+      </c>
+      <c r="I22">
+        <f>VLOOKUP($B22+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>600</v>
+      </c>
+      <c r="J22">
+        <f>VLOOKUP($B22+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1000</v>
+      </c>
+      <c r="K22">
+        <f>VLOOKUP($B22+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <f>SUM(E22:K22)/M$8</f>
+        <v>42</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="R22">
+        <f t="shared" si="6"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>12</v>
+      </c>
+      <c r="C23">
+        <f>A20</f>
+        <v>40</v>
+      </c>
+      <c r="E23">
+        <f>VLOOKUP($B23+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>400</v>
+      </c>
+      <c r="F23">
+        <f>VLOOKUP($B23+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>600</v>
+      </c>
+      <c r="G23">
+        <f>VLOOKUP($B23+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>1000</v>
+      </c>
+      <c r="H23">
+        <f>VLOOKUP($B23+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>1000</v>
+      </c>
+      <c r="I23">
+        <f>VLOOKUP($B23+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>1500</v>
+      </c>
+      <c r="J23">
+        <f>VLOOKUP($B23+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1000</v>
+      </c>
+      <c r="K23">
+        <f>VLOOKUP($B23+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f>SUM(E23:K23)/M$8</f>
+        <v>55</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="R23">
+        <f t="shared" si="6"/>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>100</v>
+      </c>
+      <c r="B24">
+        <v>13</v>
+      </c>
+      <c r="C24">
+        <f>A24</f>
+        <v>100</v>
+      </c>
+      <c r="E24">
+        <f>VLOOKUP($B24+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>400</v>
+      </c>
+      <c r="F24">
+        <f>VLOOKUP($B24+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>600</v>
+      </c>
+      <c r="G24">
+        <f>VLOOKUP($B24+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>1000</v>
+      </c>
+      <c r="H24">
+        <f>VLOOKUP($B24+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>2500</v>
+      </c>
+      <c r="I24">
+        <f>VLOOKUP($B24+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>1500</v>
+      </c>
+      <c r="J24">
+        <f>VLOOKUP($B24+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1000</v>
+      </c>
+      <c r="K24">
+        <f>VLOOKUP($B24+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f>SUM(E24:K24)/M$8</f>
+        <v>70</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="R24">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>14</v>
+      </c>
+      <c r="C25">
+        <f>A24</f>
+        <v>100</v>
+      </c>
+      <c r="E25">
+        <f>VLOOKUP($B25+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>400</v>
+      </c>
+      <c r="F25">
+        <f>VLOOKUP($B25+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>600</v>
+      </c>
+      <c r="G25">
+        <f>VLOOKUP($B25+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>2500</v>
+      </c>
+      <c r="H25">
+        <f>VLOOKUP($B25+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>2500</v>
+      </c>
+      <c r="I25">
+        <f>VLOOKUP($B25+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>1500</v>
+      </c>
+      <c r="J25">
+        <f>VLOOKUP($B25+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1000</v>
+      </c>
+      <c r="K25">
+        <f>VLOOKUP($B25+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <f>SUM(E25:K25)/M$8</f>
+        <v>85</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="R25">
+        <f t="shared" si="6"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <f>A24</f>
+        <v>100</v>
+      </c>
+      <c r="E26">
+        <f>VLOOKUP($B26+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>400</v>
+      </c>
+      <c r="F26">
+        <f>VLOOKUP($B26+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>1500</v>
+      </c>
+      <c r="G26">
+        <f>VLOOKUP($B26+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>2500</v>
+      </c>
+      <c r="H26">
+        <f>VLOOKUP($B26+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>2500</v>
+      </c>
+      <c r="I26">
+        <f>VLOOKUP($B26+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>1500</v>
+      </c>
+      <c r="J26">
+        <f>VLOOKUP($B26+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1800</v>
+      </c>
+      <c r="K26">
+        <f>VLOOKUP($B26+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <f>SUM(E26:K26)/M$8</f>
+        <v>102</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="R26">
+        <f t="shared" si="6"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <f>A24</f>
+        <v>100</v>
+      </c>
+      <c r="E27">
+        <f>VLOOKUP($B27+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1000</v>
+      </c>
+      <c r="F27">
+        <f>VLOOKUP($B27+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>1500</v>
+      </c>
+      <c r="G27">
+        <f>VLOOKUP($B27+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>2500</v>
+      </c>
+      <c r="H27">
+        <f>VLOOKUP($B27+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>2500</v>
+      </c>
+      <c r="I27">
+        <f>VLOOKUP($B27+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>2700</v>
+      </c>
+      <c r="J27">
+        <f>VLOOKUP($B27+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1800</v>
+      </c>
+      <c r="K27">
+        <f>VLOOKUP($B27+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f>SUM(E27:K27)/M$8</f>
+        <v>120</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="R27">
+        <f t="shared" si="6"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>180</v>
+      </c>
+      <c r="B28">
+        <v>17</v>
+      </c>
+      <c r="C28">
+        <f>A28</f>
+        <v>180</v>
+      </c>
+      <c r="E28">
+        <f>VLOOKUP($B28+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1000</v>
+      </c>
+      <c r="F28">
+        <f>VLOOKUP($B28+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>1500</v>
+      </c>
+      <c r="G28">
+        <f>VLOOKUP($B28+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>2500</v>
+      </c>
+      <c r="H28">
+        <f>VLOOKUP($B28+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>4500</v>
+      </c>
+      <c r="I28">
+        <f>VLOOKUP($B28+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>2700</v>
+      </c>
+      <c r="J28">
+        <f>VLOOKUP($B28+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1800</v>
+      </c>
+      <c r="K28">
+        <f>VLOOKUP($B28+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f>SUM(E28:K28)/M$8</f>
+        <v>140</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="R28">
+        <f t="shared" si="6"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>18</v>
+      </c>
+      <c r="C29">
+        <f>A28</f>
+        <v>180</v>
+      </c>
+      <c r="E29">
+        <f>VLOOKUP($B29+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1000</v>
+      </c>
+      <c r="F29">
+        <f>VLOOKUP($B29+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>1500</v>
+      </c>
+      <c r="G29">
+        <f>VLOOKUP($B29+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>4500</v>
+      </c>
+      <c r="H29">
+        <f>VLOOKUP($B29+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>4500</v>
+      </c>
+      <c r="I29">
+        <f>VLOOKUP($B29+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>2700</v>
+      </c>
+      <c r="J29">
+        <f>VLOOKUP($B29+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1800</v>
+      </c>
+      <c r="K29">
+        <f>VLOOKUP($B29+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <f>SUM(E29:K29)/M$8</f>
+        <v>160</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="6"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>19</v>
+      </c>
+      <c r="C30">
+        <f>A28</f>
+        <v>180</v>
+      </c>
+      <c r="E30">
+        <f>VLOOKUP($B30+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1000</v>
+      </c>
+      <c r="F30">
+        <f>VLOOKUP($B30+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>2700</v>
+      </c>
+      <c r="G30">
+        <f>VLOOKUP($B30+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>4500</v>
+      </c>
+      <c r="H30">
+        <f>VLOOKUP($B30+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>4500</v>
+      </c>
+      <c r="I30">
+        <f>VLOOKUP($B30+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>2700</v>
+      </c>
+      <c r="J30">
+        <f>VLOOKUP($B30+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2500</v>
+      </c>
+      <c r="K30">
+        <f>VLOOKUP($B30+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <f>SUM(E30:K30)/M$8</f>
+        <v>179</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="6"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>20</v>
+      </c>
+      <c r="C31">
+        <f>A28</f>
+        <v>180</v>
+      </c>
+      <c r="E31">
+        <f>VLOOKUP($B31+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1800</v>
+      </c>
+      <c r="F31">
+        <f>VLOOKUP($B31+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>2700</v>
+      </c>
+      <c r="G31">
+        <f>VLOOKUP($B31+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>4500</v>
+      </c>
+      <c r="H31">
+        <f>VLOOKUP($B31+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>4500</v>
+      </c>
+      <c r="I31">
+        <f>VLOOKUP($B31+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>3750</v>
+      </c>
+      <c r="J31">
+        <f>VLOOKUP($B31+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2500</v>
+      </c>
+      <c r="K31">
+        <f>VLOOKUP($B31+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <f>SUM(E31:K31)/M$8</f>
+        <v>197.5</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="5"/>
+        <v>180</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="6"/>
+        <v>197.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>250</v>
+      </c>
+      <c r="B32">
+        <v>21</v>
+      </c>
+      <c r="C32">
+        <f>A32</f>
+        <v>250</v>
+      </c>
+      <c r="E32">
+        <f>VLOOKUP($B32+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1800</v>
+      </c>
+      <c r="F32">
+        <f>VLOOKUP($B32+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>2700</v>
+      </c>
+      <c r="G32">
+        <f>VLOOKUP($B32+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>4500</v>
+      </c>
+      <c r="H32">
+        <f>VLOOKUP($B32+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>6250</v>
+      </c>
+      <c r="I32">
+        <f>VLOOKUP($B32+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>3750</v>
+      </c>
+      <c r="J32">
+        <f>VLOOKUP($B32+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2500</v>
+      </c>
+      <c r="K32">
+        <f>VLOOKUP($B32+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <f>SUM(E32:K32)/M$8</f>
+        <v>215</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="5"/>
+        <v>250</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="6"/>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>22</v>
+      </c>
+      <c r="C33">
+        <f>A32</f>
+        <v>250</v>
+      </c>
+      <c r="E33">
+        <f>VLOOKUP($B33+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1800</v>
+      </c>
+      <c r="F33">
+        <f>VLOOKUP($B33+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>2700</v>
+      </c>
+      <c r="G33">
+        <f>VLOOKUP($B33+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>6250</v>
+      </c>
+      <c r="H33">
+        <f>VLOOKUP($B33+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>6250</v>
+      </c>
+      <c r="I33">
+        <f>VLOOKUP($B33+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>3750</v>
+      </c>
+      <c r="J33">
+        <f>VLOOKUP($B33+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2500</v>
+      </c>
+      <c r="K33">
+        <f>VLOOKUP($B33+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M33">
+        <f>SUM(E33:K33)/M$8</f>
+        <v>232.5</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="5"/>
+        <v>250</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="6"/>
+        <v>232.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>23</v>
+      </c>
+      <c r="C34">
+        <f>A32</f>
+        <v>250</v>
+      </c>
+      <c r="E34">
+        <f>VLOOKUP($B34+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1800</v>
+      </c>
+      <c r="F34">
+        <f>VLOOKUP($B34+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>3750</v>
+      </c>
+      <c r="G34">
+        <f>VLOOKUP($B34+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>6250</v>
+      </c>
+      <c r="H34">
+        <f>VLOOKUP($B34+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>6250</v>
+      </c>
+      <c r="I34">
+        <f>VLOOKUP($B34+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>3750</v>
+      </c>
+      <c r="J34">
+        <f>VLOOKUP($B34+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2800</v>
+      </c>
+      <c r="K34">
+        <f>VLOOKUP($B34+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <f>SUM(E34:K34)/M$8</f>
+        <v>246</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="5"/>
+        <v>250</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="6"/>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <f>A32</f>
+        <v>250</v>
+      </c>
+      <c r="E35">
+        <f>VLOOKUP($B35+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2500</v>
+      </c>
+      <c r="F35">
+        <f>VLOOKUP($B35+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>3750</v>
+      </c>
+      <c r="G35">
+        <f>VLOOKUP($B35+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>6250</v>
+      </c>
+      <c r="H35">
+        <f>VLOOKUP($B35+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>6250</v>
+      </c>
+      <c r="I35">
+        <f>VLOOKUP($B35+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>4200</v>
+      </c>
+      <c r="J35">
+        <f>VLOOKUP($B35+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2800</v>
+      </c>
+      <c r="K35">
+        <f>VLOOKUP($B35+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <f>SUM(E35:K35)/M$8</f>
+        <v>257.5</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="5"/>
+        <v>250</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="6"/>
+        <v>257.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>280</v>
+      </c>
+      <c r="B36">
+        <v>25</v>
+      </c>
+      <c r="C36">
+        <f>A36</f>
+        <v>280</v>
+      </c>
+      <c r="E36">
+        <f>VLOOKUP($B36+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2500</v>
+      </c>
+      <c r="F36">
+        <f>VLOOKUP($B36+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>3750</v>
+      </c>
+      <c r="G36">
+        <f>VLOOKUP($B36+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>6250</v>
+      </c>
+      <c r="H36">
+        <f>VLOOKUP($B36+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>7000</v>
+      </c>
+      <c r="I36">
+        <f>VLOOKUP($B36+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>4200</v>
+      </c>
+      <c r="J36">
+        <f>VLOOKUP($B36+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2800</v>
+      </c>
+      <c r="K36">
+        <f>VLOOKUP($B36+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <f>SUM(E36:K36)/M$8</f>
+        <v>265</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="5"/>
+        <v>280</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="6"/>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>26</v>
+      </c>
+      <c r="C37">
+        <f>A36</f>
+        <v>280</v>
+      </c>
+      <c r="E37">
+        <f>VLOOKUP($B37+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2500</v>
+      </c>
+      <c r="F37">
+        <f>VLOOKUP($B37+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>3750</v>
+      </c>
+      <c r="G37">
+        <f>VLOOKUP($B37+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>7000</v>
+      </c>
+      <c r="H37">
+        <f>VLOOKUP($B37+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>7000</v>
+      </c>
+      <c r="I37">
+        <f>VLOOKUP($B37+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>4200</v>
+      </c>
+      <c r="J37">
+        <f>VLOOKUP($B37+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2800</v>
+      </c>
+      <c r="K37">
+        <f>VLOOKUP($B37+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M37">
+        <f>SUM(E37:K37)/M$8</f>
+        <v>272.5</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" si="5"/>
+        <v>280</v>
+      </c>
+      <c r="R37">
+        <f t="shared" si="6"/>
+        <v>272.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>27</v>
+      </c>
+      <c r="C38">
+        <f>A36</f>
+        <v>280</v>
+      </c>
+      <c r="E38">
+        <f>VLOOKUP($B38+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2500</v>
+      </c>
+      <c r="F38">
+        <f>VLOOKUP($B38+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>4200</v>
+      </c>
+      <c r="G38">
+        <f>VLOOKUP($B38+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>7000</v>
+      </c>
+      <c r="H38">
+        <f>VLOOKUP($B38+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>7000</v>
+      </c>
+      <c r="I38">
+        <f>VLOOKUP($B38+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>4200</v>
+      </c>
+      <c r="J38">
+        <f>VLOOKUP($B38+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2700</v>
+      </c>
+      <c r="K38">
+        <f>VLOOKUP($B38+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M38">
+        <f>SUM(E38:K38)/M$8</f>
+        <v>276</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" si="5"/>
+        <v>280</v>
+      </c>
+      <c r="R38">
+        <f t="shared" si="6"/>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>28</v>
+      </c>
+      <c r="C39">
+        <f>A36</f>
+        <v>280</v>
+      </c>
+      <c r="E39">
+        <f>VLOOKUP($B39+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2800</v>
+      </c>
+      <c r="F39">
+        <f>VLOOKUP($B39+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>4200</v>
+      </c>
+      <c r="G39">
+        <f>VLOOKUP($B39+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>7000</v>
+      </c>
+      <c r="H39">
+        <f>VLOOKUP($B39+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>7000</v>
+      </c>
+      <c r="I39">
+        <f>VLOOKUP($B39+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>4050</v>
+      </c>
+      <c r="J39">
+        <f>VLOOKUP($B39+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2700</v>
+      </c>
+      <c r="K39">
+        <f>VLOOKUP($B39+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M39">
+        <f>SUM(E39:K39)/M$8</f>
+        <v>277.5</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" si="5"/>
+        <v>280</v>
+      </c>
+      <c r="R39">
+        <f t="shared" si="6"/>
+        <v>277.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>270</v>
+      </c>
+      <c r="B40">
+        <v>29</v>
+      </c>
+      <c r="C40">
+        <f>A40</f>
+        <v>270</v>
+      </c>
+      <c r="E40">
+        <f>VLOOKUP($B40+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2800</v>
+      </c>
+      <c r="F40">
+        <f>VLOOKUP($B40+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>4200</v>
+      </c>
+      <c r="G40">
+        <f>VLOOKUP($B40+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>7000</v>
+      </c>
+      <c r="H40">
+        <f>VLOOKUP($B40+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>6750</v>
+      </c>
+      <c r="I40">
+        <f>VLOOKUP($B40+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>4050</v>
+      </c>
+      <c r="J40">
+        <f>VLOOKUP($B40+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2700</v>
+      </c>
+      <c r="K40">
+        <f>VLOOKUP($B40+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M40">
+        <f>SUM(E40:K40)/M$8</f>
+        <v>275</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" si="5"/>
+        <v>270</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="6"/>
+        <v>275</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>30</v>
+      </c>
+      <c r="C41">
+        <f>A40</f>
+        <v>270</v>
+      </c>
+      <c r="E41">
+        <f>VLOOKUP($B41+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2800</v>
+      </c>
+      <c r="F41">
+        <f>VLOOKUP($B41+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>4200</v>
+      </c>
+      <c r="G41">
+        <f>VLOOKUP($B41+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>6750</v>
+      </c>
+      <c r="H41">
+        <f>VLOOKUP($B41+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>6750</v>
+      </c>
+      <c r="I41">
+        <f>VLOOKUP($B41+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>4050</v>
+      </c>
+      <c r="J41">
+        <f>VLOOKUP($B41+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2700</v>
+      </c>
+      <c r="K41">
+        <f>VLOOKUP($B41+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M41">
+        <f>SUM(E41:K41)/M$8</f>
+        <v>272.5</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" si="5"/>
+        <v>270</v>
+      </c>
+      <c r="R41">
+        <f t="shared" si="6"/>
+        <v>272.5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B42">
+        <v>31</v>
+      </c>
+      <c r="C42">
+        <f>A40</f>
+        <v>270</v>
+      </c>
+      <c r="E42">
+        <f>VLOOKUP($B42+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2800</v>
+      </c>
+      <c r="F42">
+        <f>VLOOKUP($B42+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>4050</v>
+      </c>
+      <c r="G42">
+        <f>VLOOKUP($B42+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>6750</v>
+      </c>
+      <c r="H42">
+        <f>VLOOKUP($B42+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>6750</v>
+      </c>
+      <c r="I42">
+        <f>VLOOKUP($B42+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>4050</v>
+      </c>
+      <c r="J42">
+        <f>VLOOKUP($B42+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2100</v>
+      </c>
+      <c r="K42">
+        <f>VLOOKUP($B42+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <f>SUM(E42:K42)/M$8</f>
+        <v>265</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" si="5"/>
+        <v>270</v>
+      </c>
+      <c r="R42">
+        <f t="shared" si="6"/>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>32</v>
+      </c>
+      <c r="C43">
+        <f>A40</f>
+        <v>270</v>
+      </c>
+      <c r="E43">
+        <f>VLOOKUP($B43+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2700</v>
+      </c>
+      <c r="F43">
+        <f>VLOOKUP($B43+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>4050</v>
+      </c>
+      <c r="G43">
+        <f>VLOOKUP($B43+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>6750</v>
+      </c>
+      <c r="H43">
+        <f>VLOOKUP($B43+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>6750</v>
+      </c>
+      <c r="I43">
+        <f>VLOOKUP($B43+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>3150</v>
+      </c>
+      <c r="J43">
+        <f>VLOOKUP($B43+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2100</v>
+      </c>
+      <c r="K43">
+        <f>VLOOKUP($B43+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <f>SUM(E43:K43)/M$8</f>
+        <v>255</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" si="5"/>
+        <v>270</v>
+      </c>
+      <c r="R43">
+        <f t="shared" si="6"/>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>210</v>
+      </c>
+      <c r="B44">
+        <v>33</v>
+      </c>
+      <c r="C44">
+        <f>A44</f>
+        <v>210</v>
+      </c>
+      <c r="E44">
+        <f>VLOOKUP($B44+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2700</v>
+      </c>
+      <c r="F44">
+        <f>VLOOKUP($B44+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>4050</v>
+      </c>
+      <c r="G44">
+        <f>VLOOKUP($B44+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>6750</v>
+      </c>
+      <c r="H44">
+        <f>VLOOKUP($B44+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>5250</v>
+      </c>
+      <c r="I44">
+        <f>VLOOKUP($B44+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>3150</v>
+      </c>
+      <c r="J44">
+        <f>VLOOKUP($B44+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2100</v>
+      </c>
+      <c r="K44">
+        <f>VLOOKUP($B44+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <f>SUM(E44:K44)/M$8</f>
+        <v>240</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="R44">
+        <f t="shared" si="6"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>34</v>
+      </c>
+      <c r="C45">
+        <f>A44</f>
+        <v>210</v>
+      </c>
+      <c r="E45">
+        <f>VLOOKUP($B45+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2700</v>
+      </c>
+      <c r="F45">
+        <f>VLOOKUP($B45+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>4050</v>
+      </c>
+      <c r="G45">
+        <f>VLOOKUP($B45+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>5250</v>
+      </c>
+      <c r="H45">
+        <f>VLOOKUP($B45+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>5250</v>
+      </c>
+      <c r="I45">
+        <f>VLOOKUP($B45+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>3150</v>
+      </c>
+      <c r="J45">
+        <f>VLOOKUP($B45+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>2100</v>
+      </c>
+      <c r="K45">
+        <f>VLOOKUP($B45+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <f>SUM(E45:K45)/M$8</f>
+        <v>225</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="R45">
+        <f t="shared" si="6"/>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>35</v>
+      </c>
+      <c r="C46">
+        <f>A44</f>
+        <v>210</v>
+      </c>
+      <c r="E46">
+        <f>VLOOKUP($B46+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2700</v>
+      </c>
+      <c r="F46">
+        <f>VLOOKUP($B46+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>3150</v>
+      </c>
+      <c r="G46">
+        <f>VLOOKUP($B46+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>5250</v>
+      </c>
+      <c r="H46">
+        <f>VLOOKUP($B46+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>5250</v>
+      </c>
+      <c r="I46">
+        <f>VLOOKUP($B46+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>3150</v>
+      </c>
+      <c r="J46">
+        <f>VLOOKUP($B46+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1200</v>
+      </c>
+      <c r="K46">
+        <f>VLOOKUP($B46+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <f>SUM(E46:K46)/M$8</f>
+        <v>207</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="R46">
+        <f t="shared" si="6"/>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>36</v>
+      </c>
+      <c r="C47">
+        <f>A44</f>
+        <v>210</v>
+      </c>
+      <c r="E47">
+        <f>VLOOKUP($B47+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2100</v>
+      </c>
+      <c r="F47">
+        <f>VLOOKUP($B47+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>3150</v>
+      </c>
+      <c r="G47">
+        <f>VLOOKUP($B47+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>5250</v>
+      </c>
+      <c r="H47">
+        <f>VLOOKUP($B47+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>5250</v>
+      </c>
+      <c r="I47">
+        <f>VLOOKUP($B47+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>1800</v>
+      </c>
+      <c r="J47">
+        <f>VLOOKUP($B47+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1200</v>
+      </c>
+      <c r="K47">
+        <f>VLOOKUP($B47+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <f>SUM(E47:K47)/M$8</f>
+        <v>187.5</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" si="5"/>
+        <v>210</v>
+      </c>
+      <c r="R47">
+        <f t="shared" si="6"/>
+        <v>187.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>120</v>
+      </c>
+      <c r="B48">
+        <v>37</v>
+      </c>
+      <c r="C48">
+        <f>A48</f>
+        <v>120</v>
+      </c>
+      <c r="E48">
+        <f>VLOOKUP($B48+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2100</v>
+      </c>
+      <c r="F48">
+        <f>VLOOKUP($B48+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>3150</v>
+      </c>
+      <c r="G48">
+        <f>VLOOKUP($B48+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>5250</v>
+      </c>
+      <c r="H48">
+        <f>VLOOKUP($B48+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>3000</v>
+      </c>
+      <c r="I48">
+        <f>VLOOKUP($B48+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>1800</v>
+      </c>
+      <c r="J48">
+        <f>VLOOKUP($B48+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1200</v>
+      </c>
+      <c r="K48">
+        <f>VLOOKUP($B48+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <f>SUM(E48:K48)/M$8</f>
+        <v>165</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="R48">
+        <f t="shared" si="6"/>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>38</v>
+      </c>
+      <c r="C49">
+        <f>A48</f>
+        <v>120</v>
+      </c>
+      <c r="E49">
+        <f>VLOOKUP($B49+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2100</v>
+      </c>
+      <c r="F49">
+        <f>VLOOKUP($B49+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>3150</v>
+      </c>
+      <c r="G49">
+        <f>VLOOKUP($B49+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>3000</v>
+      </c>
+      <c r="H49">
+        <f>VLOOKUP($B49+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>3000</v>
+      </c>
+      <c r="I49">
+        <f>VLOOKUP($B49+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>1800</v>
+      </c>
+      <c r="J49">
+        <f>VLOOKUP($B49+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>1200</v>
+      </c>
+      <c r="K49">
+        <f>VLOOKUP($B49+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <f>SUM(E49:K49)/M$8</f>
+        <v>142.5</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="R49">
+        <f t="shared" si="6"/>
+        <v>142.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B50">
+        <v>39</v>
+      </c>
+      <c r="C50">
+        <f>A48</f>
+        <v>120</v>
+      </c>
+      <c r="E50">
+        <f>VLOOKUP($B50+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>2100</v>
+      </c>
+      <c r="F50">
+        <f>VLOOKUP($B50+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>1800</v>
+      </c>
+      <c r="G50">
+        <f>VLOOKUP($B50+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>3000</v>
+      </c>
+      <c r="H50">
+        <f>VLOOKUP($B50+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>3000</v>
+      </c>
+      <c r="I50">
+        <f>VLOOKUP($B50+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>1800</v>
+      </c>
+      <c r="J50">
+        <f>VLOOKUP($B50+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>200</v>
+      </c>
+      <c r="K50">
+        <f>VLOOKUP($B50+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <f>SUM(E50:K50)/M$8</f>
+        <v>119</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="R50">
+        <f t="shared" si="6"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>40</v>
+      </c>
+      <c r="C51">
+        <f>A48</f>
+        <v>120</v>
+      </c>
+      <c r="E51">
+        <f>VLOOKUP($B51+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1200</v>
+      </c>
+      <c r="F51">
+        <f>VLOOKUP($B51+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>1800</v>
+      </c>
+      <c r="G51">
+        <f>VLOOKUP($B51+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>3000</v>
+      </c>
+      <c r="H51">
+        <f>VLOOKUP($B51+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>3000</v>
+      </c>
+      <c r="I51">
+        <f>VLOOKUP($B51+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>300</v>
+      </c>
+      <c r="J51">
+        <f>VLOOKUP($B51+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>200</v>
+      </c>
+      <c r="K51">
+        <f>VLOOKUP($B51+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <f>SUM(E51:K51)/M$8</f>
+        <v>95</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" si="5"/>
+        <v>120</v>
+      </c>
+      <c r="R51">
+        <f t="shared" si="6"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>20</v>
+      </c>
+      <c r="B52">
+        <v>41</v>
+      </c>
+      <c r="C52">
+        <f>A52</f>
+        <v>20</v>
+      </c>
+      <c r="E52">
+        <f>VLOOKUP($B52+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1200</v>
+      </c>
+      <c r="F52">
+        <f>VLOOKUP($B52+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>1800</v>
+      </c>
+      <c r="G52">
+        <f>VLOOKUP($B52+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>3000</v>
+      </c>
+      <c r="H52">
+        <f>VLOOKUP($B52+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>500</v>
+      </c>
+      <c r="I52">
+        <f>VLOOKUP($B52+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>300</v>
+      </c>
+      <c r="J52">
+        <f>VLOOKUP($B52+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>200</v>
+      </c>
+      <c r="K52">
+        <f>VLOOKUP($B52+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <f>SUM(E52:K52)/M$8</f>
+        <v>70</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="Q52">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="R52">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B53">
+        <v>42</v>
+      </c>
+      <c r="C53">
+        <f>A52</f>
+        <v>20</v>
+      </c>
+      <c r="E53">
+        <f>VLOOKUP($B53+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1200</v>
+      </c>
+      <c r="F53">
+        <f>VLOOKUP($B53+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>1800</v>
+      </c>
+      <c r="G53">
+        <f>VLOOKUP($B53+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>500</v>
+      </c>
+      <c r="H53">
+        <f>VLOOKUP($B53+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>500</v>
+      </c>
+      <c r="I53">
+        <f>VLOOKUP($B53+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>300</v>
+      </c>
+      <c r="J53">
+        <f>VLOOKUP($B53+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>200</v>
+      </c>
+      <c r="K53">
+        <f>VLOOKUP($B53+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <f>SUM(E53:K53)/M$8</f>
+        <v>45</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="Q53">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="R53">
+        <f t="shared" si="6"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B54">
+        <v>43</v>
+      </c>
+      <c r="C54">
+        <f>A52</f>
+        <v>20</v>
+      </c>
+      <c r="E54">
+        <f>VLOOKUP($B54+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>1200</v>
+      </c>
+      <c r="F54">
+        <f>VLOOKUP($B54+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>300</v>
+      </c>
+      <c r="G54">
+        <f>VLOOKUP($B54+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>500</v>
+      </c>
+      <c r="H54">
+        <f>VLOOKUP($B54+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>500</v>
+      </c>
+      <c r="I54">
+        <f>VLOOKUP($B54+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>300</v>
+      </c>
+      <c r="J54">
+        <f>VLOOKUP($B54+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <f>VLOOKUP($B54+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <f>SUM(E54:K54)/M$8</f>
+        <v>28</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="Q54">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="R54">
+        <f t="shared" si="6"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B55">
+        <v>44</v>
+      </c>
+      <c r="C55">
+        <f>A52</f>
+        <v>20</v>
+      </c>
+      <c r="E55">
+        <f>VLOOKUP($B55+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>200</v>
+      </c>
+      <c r="F55">
+        <f>VLOOKUP($B55+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>300</v>
+      </c>
+      <c r="G55">
+        <f>VLOOKUP($B55+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>500</v>
+      </c>
+      <c r="H55">
+        <f>VLOOKUP($B55+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>500</v>
+      </c>
+      <c r="I55">
+        <f>VLOOKUP($B55+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <f>VLOOKUP($B55+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <f>VLOOKUP($B55+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <f>SUM(E55:K55)/M$8</f>
+        <v>15</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="Q55">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="R55">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>0</v>
+      </c>
+      <c r="B56">
+        <v>45</v>
+      </c>
+      <c r="C56">
+        <f>A56</f>
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <f>VLOOKUP($B56+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>200</v>
+      </c>
+      <c r="F56">
+        <f>VLOOKUP($B56+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>300</v>
+      </c>
+      <c r="G56">
+        <f>VLOOKUP($B56+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>500</v>
+      </c>
+      <c r="H56">
+        <f>VLOOKUP($B56+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <f>VLOOKUP($B56+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <f>VLOOKUP($B56+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <f>VLOOKUP($B56+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <f>SUM(E56:K56)/M$8</f>
+        <v>10</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="Q56">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R56">
+        <f t="shared" si="6"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="57" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B57">
+        <v>46</v>
+      </c>
+      <c r="C57">
+        <f>A56</f>
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <f>VLOOKUP($B57+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>200</v>
+      </c>
+      <c r="F57">
+        <f>VLOOKUP($B57+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>300</v>
+      </c>
+      <c r="G57">
+        <f>VLOOKUP($B57+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <f>VLOOKUP($B57+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <f>VLOOKUP($B57+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <f>VLOOKUP($B57+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <f>VLOOKUP($B57+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M57">
+        <f>SUM(E57:K57)/M$8</f>
+        <v>5</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="Q57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R57">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B58">
+        <v>47</v>
+      </c>
+      <c r="C58">
+        <f>A56</f>
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <f>VLOOKUP($B58+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>200</v>
+      </c>
+      <c r="F58">
+        <f>VLOOKUP($B58+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <f>VLOOKUP($B58+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <f>VLOOKUP($B58+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <f>VLOOKUP($B58+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <f>VLOOKUP($B58+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <f>VLOOKUP($B58+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <f>SUM(E58:K58)/M$8</f>
+        <v>2</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="Q58">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R58">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <v>48</v>
+      </c>
+      <c r="C59">
+        <f>A56</f>
+        <v>0</v>
+      </c>
+      <c r="E59">
+        <f>VLOOKUP($B59+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <f>VLOOKUP($B59+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <f>VLOOKUP($B59+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <f>VLOOKUP($B59+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <f>VLOOKUP($B59+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <f>VLOOKUP($B59+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <f>VLOOKUP($B59+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <f>SUM(E59:K59)/M$8</f>
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="Q59">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R59">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>0</v>
+      </c>
+      <c r="B60">
+        <v>49</v>
+      </c>
+      <c r="C60">
+        <f>A60</f>
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <f>VLOOKUP($B60+E$7,$B$12:$C$63,2,FALSE)*E$8</f>
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <f>VLOOKUP($B60+F$7,$B$12:$C$63,2,FALSE)*F$8</f>
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <f>VLOOKUP($B60+G$7,$B$12:$C$63,2,FALSE)*G$8</f>
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <f>VLOOKUP($B60+H$7,$B$12:$C$63,2,FALSE)*H$8</f>
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <f>VLOOKUP($B60+I$7,$B$12:$C$63,2,FALSE)*I$8</f>
+        <v>0</v>
+      </c>
+      <c r="J60">
+        <f>VLOOKUP($B60+J$7,$B$12:$C$63,2,FALSE)*J$8</f>
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <f>VLOOKUP($B60+K$7,$B$12:$C$63,2,FALSE)*K$8</f>
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <f>SUM(E60:K60)/M$8</f>
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="Q60">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="R60">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B61">
+        <v>50</v>
+      </c>
+      <c r="C61">
+        <f>A60</f>
+        <v>0</v>
+      </c>
+      <c r="P61">
+        <f t="shared" ref="P61:P63" si="7">B61</f>
+        <v>50</v>
+      </c>
+      <c r="Q61">
+        <f t="shared" ref="Q61:Q63" si="8">C61</f>
+        <v>0</v>
+      </c>
+      <c r="R61">
+        <f t="shared" ref="R61:R63" si="9">M61</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B62">
+        <v>51</v>
+      </c>
+      <c r="C62">
+        <f>A60</f>
+        <v>0</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="7"/>
+        <v>51</v>
+      </c>
+      <c r="Q62">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R62">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B63">
+        <v>52</v>
+      </c>
+      <c r="C63">
+        <f>A60</f>
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="7"/>
+        <v>52</v>
+      </c>
+      <c r="Q63">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="R63">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>